<commit_message>
Continuing Analysis and Presentation
</commit_message>
<xml_diff>
--- a/data_files/Total_cost_for_top_15_pathogens_2018_USDA.xlsx
+++ b/data_files/Total_cost_for_top_15_pathogens_2018_USDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokey\Documents\NSS\Projects\capstone_project\Foodborne_Illness\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DFD98E8-3D16-4E58-B1DB-821FC6B3BD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B62483-7A6D-4D2D-8279-A17A3B833306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D55D90D-211F-4608-8938-D849EE747D5F}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{0D55D90D-211F-4608-8938-D849EE747D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,53 +120,6 @@
     <t>Vibrio vulnificus</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Vibrio </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>non-cholera species other than</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> V. parahaemolyticus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> V. vulnificus</t>
-    </r>
-  </si>
-  <si>
     <t>Yersinia enterocolitica</t>
   </si>
   <si>
@@ -197,9 +150,35 @@
     </r>
   </si>
   <si>
+    <t>Note that this set of estimates updates USDA, Economic Research Service (ERS) 2013 estimates to 2018 by adjusting for inflation and income growth as described in the Documentation page of this website. It does not update incidence number or the number of illness outcomes. Estimates in 2013 dollars can be found in the archive on the ERS, Cost of Foodborne Illnesses Data Product website.</t>
+  </si>
+  <si>
+    <t>Source: This spreadsheet is based on: Hoffmann, Sandra, Michael Batz, J. Glenn Morris Jr.  2012.  “Annual Cost of Illness and Quality-Adjusted Life Year Losses in the United States Due to 14 Foodborne Pathogens.” J. Food Protection 75(7):1291-1302.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">non-O157 Shiga toxin-producing </t>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Escherichia coli</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O157 (STEC O157)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <i/>
@@ -224,18 +203,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Shiga toxin-producing </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Escherichia coli</t>
+      <t xml:space="preserve">Vibrio </t>
     </r>
     <r>
       <rPr>
@@ -245,14 +213,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> O157 (STEC O157)</t>
+      <t>non-cholera spp.</t>
     </r>
-  </si>
-  <si>
-    <t>Note that this set of estimates updates USDA, Economic Research Service (ERS) 2013 estimates to 2018 by adjusting for inflation and income growth as described in the Documentation page of this website. It does not update incidence number or the number of illness outcomes. Estimates in 2013 dollars can be found in the archive on the ERS, Cost of Foodborne Illnesses Data Product website.</t>
-  </si>
-  <si>
-    <t>Source: This spreadsheet is based on: Hoffmann, Sandra, Michael Batz, J. Glenn Morris Jr.  2012.  “Annual Cost of Illness and Quality-Adjusted Life Year Losses in the United States Due to 14 Foodborne Pathogens.” J. Food Protection 75(7):1291-1302.</t>
   </si>
 </sst>
 </file>
@@ -510,6 +472,951 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Cyclospora cayetanensis</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Escherichia coli (STEC non-O157)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Vibrio parahaemolyticus</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cryptosporidium spp. (all species)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Vibrio non-cholera spp.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shigella (all species)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Escherichia coli O157 (STEC O157)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yersinia enterocolitica</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vibrio vulnificus</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Clostridium perfringens</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Campylobacter spp. (all species)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Norovirus</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Listeria monocytogenes</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Toxoplasma gondii</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Salmonella (non-typhoidal species)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2571517.8543861103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31701851.858650509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45735332.035151251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58394152.170415238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81749064.260202914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159202401.65088761</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>311036907.0812763</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>313297920.48822594</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>359481556.52688539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>384277855.5749535</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2181485783.4322653</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2566984191.1498566</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3189686110.4762712</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3744008906.6322303</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4142179160.5452719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-223F-4FF6-9C85-542399FAA023}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="901633648"/>
+        <c:axId val="901628240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="901633648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="901628240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="901628240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="901633648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>89807</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>500744</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33CA921-E355-4D96-8165-CADD0D688286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,7 +1719,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A5" sqref="A5:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -823,7 +1730,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -852,194 +1759,194 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="18"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>15</v>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="29">
-        <v>845024</v>
-      </c>
-      <c r="C6" s="24">
-        <v>2181485783.4322653</v>
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>2571517.8543861103</v>
+      </c>
+      <c r="C6" s="29">
+        <v>11407.000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="29">
-        <v>965958</v>
-      </c>
-      <c r="C7" s="25">
-        <v>384277855.5749535</v>
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="25">
+        <v>31701851.858650509</v>
+      </c>
+      <c r="C7" s="29">
+        <v>112752</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="25">
+        <v>45735332.035151251</v>
+      </c>
+      <c r="C8" s="29">
+        <v>34664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B9" s="25">
+        <v>58394152.170415238</v>
+      </c>
+      <c r="C9" s="29">
         <v>57616</v>
       </c>
-      <c r="C8" s="25">
-        <v>58394152.170415238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="29">
-        <v>11407.000000000002</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2571517.8543861103</v>
-      </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="29">
-        <v>1591</v>
-      </c>
-      <c r="C10" s="25">
-        <v>3189686110.4762712</v>
+      <c r="A10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="25">
+        <v>81749064.260202914</v>
+      </c>
+      <c r="C10" s="29">
+        <v>17564</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="29">
-        <v>5461731</v>
-      </c>
-      <c r="C11" s="25">
-        <v>2566984191.1498566</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="25">
+        <v>159202401.65088761</v>
+      </c>
+      <c r="C11" s="29">
+        <v>131254</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="29">
-        <v>1027561</v>
-      </c>
-      <c r="C12" s="25">
-        <v>4142179160.5452719</v>
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="25">
+        <v>311036907.0812763</v>
+      </c>
+      <c r="C12" s="29">
+        <v>63153</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="29">
-        <v>131254</v>
-      </c>
-      <c r="C13" s="25">
-        <v>159202401.65088761</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="25">
+        <v>313297920.48822594</v>
+      </c>
+      <c r="C13" s="29">
+        <v>97656</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="29">
-        <v>63153</v>
-      </c>
-      <c r="C14" s="25">
-        <v>311036907.0812763</v>
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="25">
+        <v>359481556.52688539</v>
+      </c>
+      <c r="C14" s="29">
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="29">
-        <v>112752</v>
-      </c>
-      <c r="C15" s="25">
-        <v>31701851.858650509</v>
+      <c r="A15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="25">
+        <v>384277855.5749535</v>
+      </c>
+      <c r="C15" s="29">
+        <v>965958</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="29">
-        <v>86686</v>
-      </c>
-      <c r="C16" s="25">
-        <v>3744008906.6322303</v>
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24">
+        <v>2181485783.4322653</v>
+      </c>
+      <c r="C16" s="29">
+        <v>845024</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="29">
-        <v>34664</v>
-      </c>
-      <c r="C17" s="25">
-        <v>45735332.035151251</v>
+        <v>6</v>
+      </c>
+      <c r="B17" s="25">
+        <v>2566984191.1498566</v>
+      </c>
+      <c r="C17" s="29">
+        <v>5461731</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="29">
-        <v>96</v>
-      </c>
-      <c r="C18" s="25">
-        <v>359481556.52688539</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="29.15">
-      <c r="A19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="29">
-        <v>17564</v>
-      </c>
-      <c r="C19" s="25">
-        <v>81749064.260202914</v>
+        <v>5</v>
+      </c>
+      <c r="B18" s="25">
+        <v>3189686110.4762712</v>
+      </c>
+      <c r="C18" s="29">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="25">
+        <v>3744008906.6322303</v>
+      </c>
+      <c r="C19" s="29">
+        <v>86686</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="30">
-        <v>97656</v>
-      </c>
-      <c r="C20" s="26">
-        <v>313297920.48822594</v>
+        <v>7</v>
+      </c>
+      <c r="B20" s="26">
+        <v>4142179160.5452719</v>
+      </c>
+      <c r="C20" s="30">
+        <v>1027561</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickTop="1">
       <c r="A21" s="9"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="32">
+        <v>12</v>
+      </c>
+      <c r="B22" s="28">
         <f>SUM(B6:B20)</f>
+        <v>17571792711.736931</v>
+      </c>
+      <c r="C22" s="32">
+        <f>SUM(C6:C20)</f>
         <v>8914713</v>
-      </c>
-      <c r="C22" s="28">
-        <f>SUM(C6:C20)</f>
-        <v>17571792711.736931</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1049,7 +1956,7 @@
     </row>
     <row r="25" spans="1:12" ht="18.649999999999999" customHeight="1">
       <c r="A25" s="23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -1079,7 +1986,7 @@
     </row>
     <row r="28" spans="1:12" ht="19.850000000000001" customHeight="1">
       <c r="A28" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -1104,7 +2011,11 @@
       <c r="K29" s="21"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C20">
+    <sortCondition ref="C6:C20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>